<commit_message>
pd read excel files
</commit_message>
<xml_diff>
--- a/listings.xlsx
+++ b/listings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\WEB\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED91EA8-7B00-44E4-B23F-D2CC44C1824C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5D346F-594C-4E6C-8B28-440DBEE7613F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Exchange</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>22nd Century</t>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
   <si>
     <t>Consumer Non-Durables</t>
@@ -985,7 +982,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1031,14 +1030,14 @@
       <c r="E2">
         <v>120.628</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>2019</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1046,10 +1045,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -1061,10 +1060,10 @@
         <v>1986</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1072,10 +1071,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4">
         <v>6.15</v>
@@ -1083,14 +1082,14 @@
       <c r="E4">
         <v>139.86500000000001</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
+      <c r="F4">
+        <v>2019</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1098,10 +1097,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
       </c>
       <c r="D5">
         <v>7.22</v>
@@ -1109,14 +1108,14 @@
       <c r="E5">
         <v>67.563000000000002</v>
       </c>
-      <c r="F5" t="s">
-        <v>16</v>
+      <c r="F5">
+        <v>2019</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1124,10 +1123,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
       </c>
       <c r="D6">
         <v>13.36</v>
@@ -1135,25 +1134,25 @@
       <c r="E6">
         <v>128.84299999999999</v>
       </c>
-      <c r="F6" t="s">
-        <v>16</v>
+      <c r="F6">
+        <v>2019</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
       </c>
       <c r="D7">
         <v>25.3</v>
@@ -1161,25 +1160,25 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
-        <v>16</v>
+      <c r="F7">
+        <v>2019</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>28.86</v>
@@ -1187,25 +1186,25 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
-        <v>16</v>
+      <c r="F8">
+        <v>2019</v>
       </c>
       <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
         <v>27</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
       </c>
       <c r="D9">
         <v>17.07</v>
@@ -1217,21 +1216,21 @@
         <v>2014</v>
       </c>
       <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
         <v>31</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
       </c>
       <c r="D10">
         <v>53.1</v>
@@ -1243,21 +1242,21 @@
         <v>2013</v>
       </c>
       <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
         <v>35</v>
-      </c>
-      <c r="H10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
       </c>
       <c r="D11">
         <v>12.63</v>
@@ -1269,10 +1268,10 @@
         <v>2016</v>
       </c>
       <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
         <v>39</v>
-      </c>
-      <c r="H11" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>